<commit_message>
DP Compress the code
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">מיקום תוכנה</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast\create_forecast_basic\current</t>
+    <t xml:space="preserve">W:/Data/Forecast/Tools/forecast_git/create_forecast_basic/current</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום פלט לפי גירסא</t>
@@ -116,8 +116,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,31 +150,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.41015625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DP create fix_cbs_data_230717 folder
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -31,13 +31,16 @@
     <t xml:space="preserve">מיקום תוכנה</t>
   </si>
   <si>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast\create_forecast_basic\current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מיקום פלט לפי גירסא</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">W:/Data/Forecast/Tools/forecast_git/create_forecast_basic/current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מיקום פלט לפי גירסא</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
 </sst>
 </file>
@@ -47,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -71,6 +74,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="177"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="177"/>
     </font>
   </fonts>
@@ -116,12 +126,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -142,7 +156,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
@@ -178,7 +192,18 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" display="W:/Data/Forecast/Tools/forecast_git/create_forecast_basic/current"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - main.py, forecast.py, find_file.py - Write code that checks if there is a file that contains TAZ_V in a client folder
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -38,14 +38,24 @@
   </si>
   <si>
     <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שכבה חדשה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מיקום שכבה חדשה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -116,8 +126,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -138,41 +156,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - status_exists_for_control.py - change lines 3-4 in inputs_outputs of current forecast basic excel
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -515,7 +515,7 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -525,11 +525,7 @@
           <t>מיקום שכבה חדשה</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp\TAZ_V_‏‏check.xlsx</t>
-        </is>
-      </c>
+      <c r="B5" s="3" t="inlineStr"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="3" t="n"/>

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - from_sa_cbs_to_ta_jtmt.ipynb - change the 'taz' according 'true' of 'false' in 'inputs_outputs' excel
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -131,7 +131,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,7 +159,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -197,7 +197,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - emp_current_year_230718.ipynb - change lines 3-5 in inputs_outputs of current forecast basic excel
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -472,10 +472,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.37890625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
@@ -516,35 +516,47 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp</t>
+          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="5">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>שכבה חדשה</t>
-        </is>
-      </c>
-      <c r="B4" s="7" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>מיקום פלט</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp</t>
         </is>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" s="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
+          <t>שכבה חדשה</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1" s="5">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
           <t>מיקום שכבה חדשה</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp\TAZ_V4_230518_Published.shp</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="5"/>
+    <row r="10" ht="13.5" customHeight="1" s="5"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
GK: correcting output to fit models format
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -19,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -29,26 +28,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <charset val="1"/>
-      <family val="0"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
@@ -70,48 +50,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -468,92 +420,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.37890625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.3984375" defaultRowHeight="13.8"/>
   <cols>
-    <col width="24.38" customWidth="1" style="4" min="1" max="1"/>
-    <col width="51.62" customWidth="1" style="4" min="2" max="2"/>
+    <col width="24.3984375" customWidth="1" min="1" max="1"/>
+    <col width="51.59765625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="5">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>discription</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>location</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1" s="5">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>מיקום תוכנת תחזית בסיס</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast\create_forecast_basic\current</t>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="5">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="inlineStr">
         <is>
           <t>מיקום פלט לפי גירסא</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1" s="5">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>מיקום פלט</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" s="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" t="inlineStr">
         <is>
           <t>שכבה חדשה</t>
         </is>
       </c>
-      <c r="B5" s="7" t="b">
+      <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="5">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" t="inlineStr">
         <is>
           <t>מיקום שכבה חדשה</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
     </row>
-    <row r="10" ht="13.5" customHeight="1" s="5"/>
+    <row r="10" ht="13.5" customHeight="1"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DP: create_forecast_basic current - palestinian_from_demo_230622.ipynb - change TAZ_V4 input date
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAZ_V4_date</t>
   </si>
 </sst>
 </file>
@@ -136,16 +139,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,62 +176,70 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.40234375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>240404</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
GK: small changes in ad hoc
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>c:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
+          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GK: run code determinig
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -1,41 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2074A7-C309-4B3C-B27E-1F76D79C3658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2010" yWindow="4020" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>discription</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>מיקום תוכנת תחזית בסיס</t>
+  </si>
+  <si>
+    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
+  </si>
+  <si>
+    <t>מיקום פלט לפי גירסא</t>
+  </si>
+  <si>
+    <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+  </si>
+  <si>
+    <t>מיקום פלט</t>
+  </si>
+  <si>
+    <t>שכבה חדשה</t>
+  </si>
+  <si>
+    <t>מיקום שכבה חדשה</t>
+  </si>
+  <si>
+    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\background_files\TAZ_V4_240408_with_geo_info.shp</t>
+  </si>
+  <si>
+    <t>TAZ_V4_date</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,84 +98,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -451,106 +436,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.375" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="24.375" customWidth="1" min="1" max="1"/>
-    <col width="51.625" customWidth="1" min="2" max="2"/>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="2" max="2" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>discription</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>מיקום תוכנת תחזית בסיס</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>מיקום פלט לפי גירסא</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>מיקום פלט</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>שכבה חדשה</t>
-        </is>
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>מיקום שכבה חדשה</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\background_files\TAZ_V4_240408_with_geo_info.shp</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TAZ_V4_date</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>240404</v>
-      </c>
-    </row>
-    <row r="10" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>240408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GK: fix bug in current add geo info in district field
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -1,85 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2074A7-C309-4B3C-B27E-1F76D79C3658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="4020" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2010" yWindow="4020" windowWidth="21600" windowHeight="12645" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>discription</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>מיקום תוכנת תחזית בסיס</t>
-  </si>
-  <si>
-    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
-  </si>
-  <si>
-    <t>מיקום פלט לפי גירסא</t>
-  </si>
-  <si>
-    <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
-  </si>
-  <si>
-    <t>מיקום פלט</t>
-  </si>
-  <si>
-    <t>שכבה חדשה</t>
-  </si>
-  <si>
-    <t>מיקום שכבה חדשה</t>
-  </si>
-  <si>
-    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\background_files\TAZ_V4_240408_with_geo_info.shp</t>
-  </si>
-  <si>
-    <t>TAZ_V4_date</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -98,25 +54,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -436,78 +451,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="24.375" customWidth="1"/>
-    <col min="2" max="2" width="51.625" customWidth="1"/>
+    <col width="24.375" customWidth="1" min="1" max="1"/>
+    <col width="51.625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>discription</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>מיקום תוכנת תחזית בסיס</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>מיקום פלט לפי גירסא</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>מיקום פלט</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>שכבה חדשה</t>
+        </is>
       </c>
       <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>מיקום שכבה חדשה</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\background_files\TAZ_V4_240408_with_geo_info.shp</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TAZ_V4_date</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>240408</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "GK: small changes in ad hoc"
This reverts commit f827abf134df811f4d899313f31ef394fab9cde8.
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
+          <t>c:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
DP: create_forecast_ad_hoc - change_Muni_Heb_to_Muni_Eng
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/inputs_outputs.xlsx
+++ b/create_forecast_basic/current/inputs_outputs.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
+          <t>C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
         </is>
       </c>
     </row>

</xml_diff>